<commit_message>
First Methodology Draft Submitted to Mentor, Results of Hybrid model with different stopwords combinations
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e55a912db83fd400/Desktop/DissertationRepository2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86F63488-D906-4AF5-8AC9-E2DC58F1EE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="8_{86F63488-D906-4AF5-8AC9-E2DC58F1EE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECA1B5A9-F410-4603-A6A3-5BC082280CEF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5640" windowWidth="23652" windowHeight="12492" xr2:uid="{A326EF4F-025B-49C9-9E5D-93C75AC21594}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A326EF4F-025B-49C9-9E5D-93C75AC21594}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="No stopwords" sheetId="1" r:id="rId1"/>
+    <sheet name="LSTM+CNN " sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'No stopwords'!$A$1:$B$82</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="115">
   <si>
     <t>Validation accuracy: 0.7764 with hyperparameters: {'num_filters': 128.0, 'pool_size': 4.0, 'lstm_out': 256.0, 'dropout_rate': 0.4}</t>
   </si>
@@ -267,16 +268,146 @@
   </si>
   <si>
     <t>Filters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation accuracy: 0.8331 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation accuracy: 0.8319 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation accuracy: 0.8317 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation accuracy: 0.8314 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation accuracy: 0.8312 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation accuracy: 0.8311 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation accuracy: 0.8309 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation accuracy: 0.8306 </t>
+  </si>
+  <si>
+    <t>hyperparameters: {'num_filters': 256.0, 'pool_size': 2.0, 'lstm_out': 448.0, 'dropout_rate': 0.2}</t>
+  </si>
+  <si>
+    <t>hyperparameters: {'num_filters': 256.0, 'pool_size': 2.0, 'lstm_out': 448.0, 'dropout_rate': 0.4}</t>
+  </si>
+  <si>
+    <t>hyperparameters: {'num_filters': 256.0, 'pool_size': 2.0, 'lstm_out': 384.0, 'dropout_rate': 0.2}</t>
+  </si>
+  <si>
+    <t>hyperparameters: {'num_filters': 192.0, 'pool_size': 2.0, 'lstm_out': 384.0, 'dropout_rate': 0.2}</t>
+  </si>
+  <si>
+    <t>hyperparameters: {'num_filters': 256.0, 'pool_size': 2.0, 'lstm_out': 320.0, 'dropout_rate': 0.2}</t>
+  </si>
+  <si>
+    <t>hyperparameters: {'num_filters': 192.0, 'pool_size': 2.0, 'lstm_out': 384.0, 'dropout_rate': 0.3}</t>
+  </si>
+  <si>
+    <t>hyperparameters: {'num_filters': 192.0, 'pool_size': 2.0, 'lstm_out': 512.0, 'dropout_rate': 0.2}</t>
+  </si>
+  <si>
+    <t>hyperparameters: {'num_filters': 256.0, 'pool_size': 2.0, 'lstm_out': 512.0, 'dropout_rate': 0.4}</t>
+  </si>
+  <si>
+    <t>Validation Accuracy with no stopwords</t>
+  </si>
+  <si>
+    <t>1. No stopwords</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1-Score</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>Test Accuracy with no stopwords</t>
+  </si>
+  <si>
+    <t>0.8336 (cnntlstm_modelSP2.pth)</t>
+  </si>
+  <si>
+    <t>hyperparameters: {'num_filters': 256.0, 'pool_size': 2.0, 'lstm_out': 512.0, 'dropout_rate': 0.2}</t>
+  </si>
+  <si>
+    <t>Test accuracy with stopwords</t>
+  </si>
+  <si>
+    <t>1. Stopwords</t>
+  </si>
+  <si>
+    <t>Confusion Matrix</t>
+  </si>
+  <si>
+    <t>Test accuracy with customized stopwords</t>
+  </si>
+  <si>
+    <t>1. Customized Stopwords</t>
+  </si>
+  <si>
+    <t>[46098 1259 5885]</t>
+  </si>
+  <si>
+    <t>[ 2342 43061 7918]</t>
+  </si>
+  <si>
+    <t>[ 6572 5899 40491]]</t>
+  </si>
+  <si>
+    <t>hyperparameters: {'num_filters': 192.0, 'pool_size': 2.0, 'lstm_out': 448.0, 'dropout_rate': 0.2}</t>
+  </si>
+  <si>
+    <t>[45845 2064 5307]</t>
+  </si>
+  <si>
+    <t>[ 3191 42577 7433]</t>
+  </si>
+  <si>
+    <t>[ 7522 6109 39477]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -302,8 +433,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -319,6 +459,51 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D3C31178-0204-43D4-BBF7-4624A7F4813E}" name="Table1" displayName="Table1" ref="A13:D16" totalsRowShown="0">
+  <autoFilter ref="A13:D16" xr:uid="{D3C31178-0204-43D4-BBF7-4624A7F4813E}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{46C5FD8A-59A0-4DBA-8DA5-D255D77D3553}" name="1. No stopwords"/>
+    <tableColumn id="2" xr3:uid="{6B50C29A-C459-4627-AB89-80D9F951DB12}" name="Precision"/>
+    <tableColumn id="3" xr3:uid="{3DD39FAC-C3AD-4CFC-86B8-95DDD837458C}" name="Recall"/>
+    <tableColumn id="4" xr3:uid="{E2B703E8-A2BB-4945-9268-1491D4EF16E1}" name="F1-Score"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2CAEF637-5C76-4C00-B650-F763C988992F}" name="Table13" displayName="Table13" ref="A18:E21" totalsRowShown="0">
+  <autoFilter ref="A18:E21" xr:uid="{2CAEF637-5C76-4C00-B650-F763C988992F}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{3BB15334-2468-4CAB-A7B5-EC9C6364188A}" name="1. Stopwords"/>
+    <tableColumn id="2" xr3:uid="{DF1298AE-AC5E-4742-98FF-C4417B94F18B}" name="Precision"/>
+    <tableColumn id="3" xr3:uid="{346167F3-11A6-4882-83C6-39A12161D305}" name="Recall"/>
+    <tableColumn id="4" xr3:uid="{EB72E3BD-6563-485D-984E-F008E5EE7268}" name="F1-Score"/>
+    <tableColumn id="6" xr3:uid="{9ABDA0FC-216B-4C0A-B1B6-A03AB41B8079}" name="Confusion Matrix"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE4E72C9-9A50-4C0E-B253-6355A1432BCA}" name="Table134" displayName="Table134" ref="A23:E26" totalsRowShown="0">
+  <autoFilter ref="A23:E26" xr:uid="{FE4E72C9-9A50-4C0E-B253-6355A1432BCA}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2ABC8825-B108-4CB6-A054-E73271DBD5CB}" name="1. Customized Stopwords"/>
+    <tableColumn id="2" xr3:uid="{14B42064-919C-4EDE-867D-B3A9D66FB2C3}" name="Precision"/>
+    <tableColumn id="3" xr3:uid="{AE421E05-86C7-44E1-8F67-127D2D878523}" name="Recall"/>
+    <tableColumn id="4" xr3:uid="{5D6850B9-4062-44E5-B53B-9FA57D5509F3}" name="F1-Score"/>
+    <tableColumn id="6" xr3:uid="{E23B7BC3-1244-4408-92D5-5A79226FB2D6}" name="Confusion Matrix"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -620,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E14C50-A46E-402F-9F78-1B8A2124808D}">
   <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A74" sqref="A2:A74"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,4 +1235,411 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D2834E-803B-4BED-8913-7013A397B38A}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.21875" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5546875" customWidth="1"/>
+    <col min="5" max="5" width="47.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.81269999999999998</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.80169999999999997</v>
+      </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.83179999999999998</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.81479999999999997</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.79859999999999998</v>
+      </c>
+      <c r="E3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.80189999999999995</v>
+      </c>
+      <c r="E4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.83140000000000003</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.81420000000000003</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.80189999999999995</v>
+      </c>
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.8276</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.81479999999999997</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.80610000000000004</v>
+      </c>
+      <c r="E6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.82769999999999999</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.81579999999999997</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.8034</v>
+      </c>
+      <c r="E7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.82379999999999998</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.81220000000000003</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.83209999999999995</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.81459999999999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.79879999999999995</v>
+      </c>
+      <c r="E9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.83250000000000002</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.81379999999999997</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.80410000000000004</v>
+      </c>
+      <c r="E10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.82979999999999998</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.81369999999999998</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.80220000000000002</v>
+      </c>
+      <c r="E11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14">
+        <v>0.84</v>
+      </c>
+      <c r="C14">
+        <v>0.9</v>
+      </c>
+      <c r="D14">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15">
+        <v>0.84</v>
+      </c>
+      <c r="C15">
+        <v>0.87</v>
+      </c>
+      <c r="D15">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16">
+        <v>0.81</v>
+      </c>
+      <c r="C16">
+        <v>0.74</v>
+      </c>
+      <c r="D16">
+        <v>0.77</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19">
+        <v>0.81</v>
+      </c>
+      <c r="C19">
+        <v>0.86</v>
+      </c>
+      <c r="D19">
+        <v>0.84</v>
+      </c>
+      <c r="E19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20">
+        <v>0.84</v>
+      </c>
+      <c r="C20">
+        <v>0.8</v>
+      </c>
+      <c r="D20">
+        <v>0.82</v>
+      </c>
+      <c r="E20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21">
+        <v>0.76</v>
+      </c>
+      <c r="C21">
+        <v>0.74</v>
+      </c>
+      <c r="D21">
+        <v>0.75</v>
+      </c>
+      <c r="E21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24">
+        <v>0.84</v>
+      </c>
+      <c r="C24">
+        <v>0.87</v>
+      </c>
+      <c r="D24">
+        <v>0.85</v>
+      </c>
+      <c r="E24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25">
+        <v>0.86</v>
+      </c>
+      <c r="C25">
+        <v>0.81</v>
+      </c>
+      <c r="D25">
+        <v>0.83</v>
+      </c>
+      <c r="E25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26">
+        <v>0.75</v>
+      </c>
+      <c r="C26">
+        <v>0.76</v>
+      </c>
+      <c r="D26">
+        <v>0.76</v>
+      </c>
+      <c r="E26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Overleaf Template & Updated VADER Implementation
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clayt\OneDrive\Desktop\DissertationRepository2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e55a912db83fd400/Desktop/DissertationRepository2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A75A75-A1C4-41E4-9CF4-DBE1A6C1BAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{A9A75A75-A1C4-41E4-9CF4-DBE1A6C1BAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A57CFC46-7E64-4703-830E-43A7636BC831}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{A326EF4F-025B-49C9-9E5D-93C75AC21594}"/>
+    <workbookView xWindow="49620" yWindow="645" windowWidth="23010" windowHeight="12330" xr2:uid="{A326EF4F-025B-49C9-9E5D-93C75AC21594}"/>
   </bookViews>
   <sheets>
-    <sheet name="No stopwords + LSTM" sheetId="1" r:id="rId1"/>
-    <sheet name="LSTM+CNN " sheetId="2" r:id="rId2"/>
-    <sheet name="No stopwords TFIDF" sheetId="3" r:id="rId3"/>
-    <sheet name="TF-IDF" sheetId="4" r:id="rId4"/>
-    <sheet name="No stopwords NB" sheetId="5" r:id="rId5"/>
-    <sheet name="BoW" sheetId="6" r:id="rId6"/>
+    <sheet name="VADER" sheetId="7" r:id="rId1"/>
+    <sheet name="No stopwords + LSTM" sheetId="1" r:id="rId2"/>
+    <sheet name="LSTM+CNN " sheetId="2" r:id="rId3"/>
+    <sheet name="No stopwords TFIDF" sheetId="3" r:id="rId4"/>
+    <sheet name="TF-IDF" sheetId="4" r:id="rId5"/>
+    <sheet name="No stopwords NB" sheetId="5" r:id="rId6"/>
+    <sheet name="BoW" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'No stopwords + LSTM'!$A$1:$B$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'No stopwords + LSTM'!$A$1:$B$82</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="940">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="944">
   <si>
     <t>Validation accuracy: 0.7764 with hyperparameters: {'num_filters': 128.0, 'pool_size': 4.0, 'lstm_out': 256.0, 'dropout_rate': 0.4}</t>
   </si>
@@ -2864,6 +2865,18 @@
   </si>
   <si>
     <t>[[47570 1405 4390] [ 1753 45642 5578] [ 6514 6759 39915]]</t>
+  </si>
+  <si>
+    <t>Accuracy: 61.65%</t>
+  </si>
+  <si>
+    <t>Accuracy 61.14%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Removing stopwords </t>
+  </si>
+  <si>
+    <t>1. Custom Stopwords</t>
   </si>
 </sst>
 </file>
@@ -2991,7 +3004,78 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C270D486-B562-4660-9CF3-D71B4B5BB641}" name="Table110" displayName="Table110" ref="A1:D5" totalsRowShown="0">
+  <autoFilter ref="A1:D5" xr:uid="{C270D486-B562-4660-9CF3-D71B4B5BB641}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{07B7FED2-5BD7-4198-AEA6-E4B58008C991}" name="1. Removing stopwords "/>
+    <tableColumn id="2" xr3:uid="{30F0CEF1-FBF2-4714-965F-5B512E66D534}" name="Precision"/>
+    <tableColumn id="3" xr3:uid="{B4EF25E1-0BB0-4EAE-B19E-7372DB6399C4}" name="Recall"/>
+    <tableColumn id="4" xr3:uid="{14D0EADA-3D92-4EF8-BCFA-6AF687001F29}" name="F1-Score"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{61391C26-6CA8-499D-949D-0E36741730A4}" name="Table1578" displayName="Table1578" ref="A18:E21" totalsRowShown="0">
+  <autoFilter ref="A18:E21" xr:uid="{61391C26-6CA8-499D-949D-0E36741730A4}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{C8512047-4401-49E3-A904-8B24628A6495}" name="1. Customized stopwords"/>
+    <tableColumn id="2" xr3:uid="{A337DE6D-CD0F-4438-824F-4783B71AE6A1}" name="Precision"/>
+    <tableColumn id="3" xr3:uid="{40E39733-E8CB-4083-8DAB-A3C92C698C33}" name="Recall"/>
+    <tableColumn id="4" xr3:uid="{D9182BF1-03B0-4BB1-8178-C5A5E2F1A989}" name="F1-Score"/>
+    <tableColumn id="5" xr3:uid="{49C50D54-738E-41AE-9DCF-7E1085FC56DB}" name="Confusion Matrix"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A5D144CF-5007-4CD7-9E64-E1413FCE741E}" name="Table15789" displayName="Table15789" ref="A23:E26" totalsRowShown="0">
+  <autoFilter ref="A23:E26" xr:uid="{A5D144CF-5007-4CD7-9E64-E1413FCE741E}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{20DB14C9-728A-46C9-91A6-67365301F52E}" name="1. No stopwords"/>
+    <tableColumn id="2" xr3:uid="{EA49F63D-B9A6-4999-B606-FF18CB2FED97}" name="Precision"/>
+    <tableColumn id="3" xr3:uid="{0B6B9593-A937-4C5C-8AA4-1CFAC26D40AE}" name="Recall"/>
+    <tableColumn id="4" xr3:uid="{AF632AA9-64A4-4165-8040-7F3C7C812967}" name="F1-Score"/>
+    <tableColumn id="5" xr3:uid="{D0C775AE-4BF7-41FB-86A3-86470A46C7EF}" name="Confusion Matrix"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{18215F79-D788-42C9-9753-1DDD9CB2A763}" name="Table11011" displayName="Table11011" ref="A7:D11" totalsRowShown="0">
+  <autoFilter ref="A7:D11" xr:uid="{18215F79-D788-42C9-9753-1DDD9CB2A763}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{089734D3-069E-4298-97FC-092A6F741C4F}" name="1. Stopwords"/>
+    <tableColumn id="2" xr3:uid="{F6F5DC7E-F108-4961-BA7F-5D700A4C8E90}" name="Precision"/>
+    <tableColumn id="3" xr3:uid="{F25574E2-CE65-45B4-8C8F-440296D948BF}" name="Recall"/>
+    <tableColumn id="4" xr3:uid="{AEB96417-9EE4-4BE1-A842-497A61EE544C}" name="F1-Score"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3B934533-BD06-4422-80F4-D7BDD3487DD4}" name="Table1101112" displayName="Table1101112" ref="A13:D17" totalsRowShown="0">
+  <autoFilter ref="A13:D17" xr:uid="{3B934533-BD06-4422-80F4-D7BDD3487DD4}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{9E75E3D0-22EE-44B7-8814-664A41F4EFDC}" name="1. Custom Stopwords"/>
+    <tableColumn id="2" xr3:uid="{1F56D721-6ABD-4A45-98C8-4CCDA0045020}" name="Precision"/>
+    <tableColumn id="3" xr3:uid="{DF6305FD-54D7-447A-84D0-C737AACBB982}" name="Recall"/>
+    <tableColumn id="4" xr3:uid="{124DDE92-946A-4A6B-A51B-7C8E2CB2E87E}" name="F1-Score"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D3C31178-0204-43D4-BBF7-4624A7F4813E}" name="Table1" displayName="Table1" ref="A13:D16" totalsRowShown="0">
   <autoFilter ref="A13:D16" xr:uid="{D3C31178-0204-43D4-BBF7-4624A7F4813E}"/>
   <tableColumns count="4">
@@ -3004,7 +3088,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2CAEF637-5C76-4C00-B650-F763C988992F}" name="Table13" displayName="Table13" ref="A18:E21" totalsRowShown="0">
   <autoFilter ref="A18:E21" xr:uid="{2CAEF637-5C76-4C00-B650-F763C988992F}"/>
   <tableColumns count="5">
@@ -3018,7 +3102,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE4E72C9-9A50-4C0E-B253-6355A1432BCA}" name="Table134" displayName="Table134" ref="A23:E26" totalsRowShown="0">
   <autoFilter ref="A23:E26" xr:uid="{FE4E72C9-9A50-4C0E-B253-6355A1432BCA}"/>
   <tableColumns count="5">
@@ -3032,7 +3116,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{56C14F18-0B6D-4DB3-B1CA-5FCEDC8BDC81}" name="Table15" displayName="Table15" ref="A13:E16" totalsRowShown="0">
   <autoFilter ref="A13:E16" xr:uid="{56C14F18-0B6D-4DB3-B1CA-5FCEDC8BDC81}"/>
   <tableColumns count="5">
@@ -3046,7 +3130,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{40699ED9-C8C5-4F67-A05D-ED8192DC45A9}" name="Table156" displayName="Table156" ref="A18:E22" totalsRowShown="0">
   <autoFilter ref="A18:E22" xr:uid="{40699ED9-C8C5-4F67-A05D-ED8192DC45A9}"/>
   <tableColumns count="5">
@@ -3060,7 +3144,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5B987CA1-92CE-426B-873E-67C2688F9282}" name="Table157" displayName="Table157" ref="A13:E16" totalsRowShown="0">
   <autoFilter ref="A13:E16" xr:uid="{5B987CA1-92CE-426B-873E-67C2688F9282}"/>
   <tableColumns count="5">
@@ -3069,34 +3153,6 @@
     <tableColumn id="3" xr3:uid="{50B25DA4-42AE-4825-8320-1B88C59FF274}" name="Recall"/>
     <tableColumn id="4" xr3:uid="{1FDEE4D8-151A-45F2-94EA-8291193773C5}" name="F1-Score"/>
     <tableColumn id="5" xr3:uid="{3AAE7D9A-76A0-43A4-B5C2-78443561AC56}" name="Confusion Matrix"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{61391C26-6CA8-499D-949D-0E36741730A4}" name="Table1578" displayName="Table1578" ref="A18:E21" totalsRowShown="0">
-  <autoFilter ref="A18:E21" xr:uid="{61391C26-6CA8-499D-949D-0E36741730A4}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C8512047-4401-49E3-A904-8B24628A6495}" name="1. Customized stopwords"/>
-    <tableColumn id="2" xr3:uid="{A337DE6D-CD0F-4438-824F-4783B71AE6A1}" name="Precision"/>
-    <tableColumn id="3" xr3:uid="{40E39733-E8CB-4083-8DAB-A3C92C698C33}" name="Recall"/>
-    <tableColumn id="4" xr3:uid="{D9182BF1-03B0-4BB1-8178-C5A5E2F1A989}" name="F1-Score"/>
-    <tableColumn id="5" xr3:uid="{49C50D54-738E-41AE-9DCF-7E1085FC56DB}" name="Confusion Matrix"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A5D144CF-5007-4CD7-9E64-E1413FCE741E}" name="Table15789" displayName="Table15789" ref="A23:E26" totalsRowShown="0">
-  <autoFilter ref="A23:E26" xr:uid="{A5D144CF-5007-4CD7-9E64-E1413FCE741E}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{20DB14C9-728A-46C9-91A6-67365301F52E}" name="1. No stopwords"/>
-    <tableColumn id="2" xr3:uid="{EA49F63D-B9A6-4999-B606-FF18CB2FED97}" name="Precision"/>
-    <tableColumn id="3" xr3:uid="{0B6B9593-A937-4C5C-8AA4-1CFAC26D40AE}" name="Recall"/>
-    <tableColumn id="4" xr3:uid="{AF632AA9-64A4-4165-8040-7F3C7C812967}" name="F1-Score"/>
-    <tableColumn id="5" xr3:uid="{D0C775AE-4BF7-41FB-86A3-86470A46C7EF}" name="Confusion Matrix"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3398,6 +3454,218 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F88775-41E5-4883-ADA3-E4FA8EBD55A2}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="A1:D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>942</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2">
+        <v>0.72</v>
+      </c>
+      <c r="C2">
+        <v>0.65</v>
+      </c>
+      <c r="D2">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3">
+        <v>0.54</v>
+      </c>
+      <c r="C3">
+        <v>0.87</v>
+      </c>
+      <c r="D3">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4">
+        <v>0.67</v>
+      </c>
+      <c r="C4">
+        <v>0.32</v>
+      </c>
+      <c r="D4">
+        <v>0.43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8">
+        <v>0.71</v>
+      </c>
+      <c r="C8">
+        <v>0.65</v>
+      </c>
+      <c r="D8">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9">
+        <v>0.54</v>
+      </c>
+      <c r="C9">
+        <v>0.87</v>
+      </c>
+      <c r="D9">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10">
+        <v>0.67</v>
+      </c>
+      <c r="C10">
+        <v>0.31</v>
+      </c>
+      <c r="D10">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>943</v>
+      </c>
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14">
+        <v>0.7</v>
+      </c>
+      <c r="C14">
+        <v>0.65</v>
+      </c>
+      <c r="D14">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15">
+        <v>0.54</v>
+      </c>
+      <c r="C15">
+        <v>0.86</v>
+      </c>
+      <c r="D15">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16">
+        <v>0.67</v>
+      </c>
+      <c r="C16">
+        <v>0.32</v>
+      </c>
+      <c r="D16">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>941</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E14C50-A46E-402F-9F78-1B8A2124808D}">
   <dimension ref="A1:B82"/>
   <sheetViews>
@@ -3833,12 +4101,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D2834E-803B-4BED-8913-7013A397B38A}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4243,7 +4511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633E71A7-67C4-4D87-BF7E-9B80821C1D57}">
   <dimension ref="A1:B384"/>
   <sheetViews>
@@ -7337,7 +7605,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FEAA5D-0F88-48A6-9636-331A8258A080}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -7757,7 +8025,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B709C1-145D-4A0F-B316-299F2FA790E0}">
   <dimension ref="A1:B82"/>
   <sheetViews>
@@ -8429,7 +8697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BEEFC2-1DF8-4A8F-8685-74C9C04A1756}">
   <dimension ref="A1:E26"/>
   <sheetViews>

</xml_diff>